<commit_message>
Review the solution for correctness
</commit_message>
<xml_diff>
--- a/CH-92 Missing value.xlsx
+++ b/CH-92 Missing value.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4FCCF9-D00B-431D-8CAC-CF1AF3C524E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A052171-80AA-4ECC-BD7F-67010FFCD0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="14">
   <si>
     <t>Question</t>
   </si>
@@ -98,6 +98,15 @@
   <si>
     <t>I like the offset approach for its obvious approach.</t>
   </si>
+  <si>
+    <t>Switch is not a bad approach for this.</t>
+  </si>
+  <si>
+    <t>Not much different than IFS. Just different, not better.</t>
+  </si>
+  <si>
+    <t>One issue with offset is that it is volatile. This means it recomputes on every change, which is not necessary.</t>
+  </si>
 </sst>
 </file>
 
@@ -106,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +156,13 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Corbel"/>
       <family val="2"/>
@@ -245,7 +261,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -266,14 +282,15 @@
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Intro_Hd" xfId="2" xr:uid="{939452B0-992F-464A-8BB9-90FACA3DA973}"/>
@@ -897,22 +914,22 @@
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="14"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -5485,22 +5502,22 @@
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="14"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -10218,7 +10235,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I19:I20"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10235,22 +10252,22 @@
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="14"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -14906,8 +14923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04079D5C-BDC8-4765-B8EC-A1D20E64C238}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14924,22 +14941,22 @@
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="14"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -15455,7 +15472,7 @@
       <c r="S15" s="9"/>
     </row>
     <row r="16" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="7"/>
@@ -15508,6 +15525,9 @@
         <f ca="1"/>
         <v>1</v>
       </c>
+      <c r="M18" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="P18" s="8"/>
       <c r="S18" s="9"/>
     </row>
@@ -15544,6 +15564,9 @@
         <f ca="1"/>
         <v>1</v>
       </c>
+      <c r="M19" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="P19" s="8"/>
       <c r="S19" s="9"/>
     </row>
@@ -15615,6 +15638,9 @@
       <c r="K21" t="b">
         <f ca="1"/>
         <v>1</v>
+      </c>
+      <c r="M21" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="P21" s="8"/>
       <c r="S21" s="9"/>

</xml_diff>

<commit_message>
Another Interim Index solution
</commit_message>
<xml_diff>
--- a/CH-92 Missing value.xlsx
+++ b/CH-92 Missing value.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B09CD5B-7940-4F91-89BB-7F863363DDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D284A7E-211F-414D-979A-055A89E029FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,8 +44,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -56,11 +57,35 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="2">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
@@ -706,6 +731,72 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <v>13</v>
+    <v>2</v>
+  </rv>
+  <rv s="1">
+    <v>13</v>
+    <v>1</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="propagated" t="b"/>
+  </s>
+</rvStructures>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -19868,8 +19959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A932BE-8E3C-470C-A0EC-77638493AE59}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -20431,35 +20522,32 @@
       <c r="S17" s="9"/>
     </row>
     <row r="18" spans="3:19" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C18" s="3" cm="1">
-        <f t="array" aca="1" ref="C18" ca="1">_xlfn.VSTACK(K2:N2,_xlfn.MAP(
+      <c r="C18" s="3" t="e" cm="1" vm="1">
+        <f t="array" ref="C18">_xlfn.VSTACK(K2:N2,_xlfn.MAP(
 C3:F12,
-_xlfn.LAMBDA(_xlpm.v,  _xlfn.LET(_xlpm.r, _xlfn.IFS(_xlpm.v="U",-1,_xlpm.v="D",1,1,0),
-               _xlpm.c, _xlfn.IFS(_xlpm.v="L",-1,_xlpm.v="R",1,1,0),
-               _xlpm.z, INDEX(_xlfn.ANCHORARRAY($C$18),ROW(_xlpm.v)+_xlpm.r-ROW($C$18)+1,COLUMN(_xlpm.v)+_xlpm.c-COLUMN($C$18)+1),
-               _xlpm.z)
-      )
-))</f>
-        <v>0</v>
+_xlfn.LAMBDA(_xlpm.v,_xlfn.LET(_xlpm.r,_xlfn.IFS(_xlpm.v="U",-1,_xlpm.v="D",1,1,0),
+_xlpm.c,_xlfn.IFS(_xlpm.v="L",-1,_xlpm.v="R",1,1,0),
+_xlpm.z,INDEX(_xlpm.v,1,1):INDEX(_xlpm.v,1,1),
+INDEX($C$3:$F$12,ROW(_xlpm.z)+_xlpm.r-3,COLUMN(_xlpm.z)+_xlpm.c-3)
+)
+)))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="H18" t="b" cm="1">
-        <f t="array" aca="1" ref="H18:K28" ca="1">_xlfn.ANCHORARRAY(C18)=K2:N12</f>
-        <v>1</v>
-      </c>
-      <c r="I18" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J18" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K18" t="b">
-        <f ca="1"/>
-        <v>1</v>
+      <c r="H18" t="e" cm="1" vm="2">
+        <f t="array" ref="H18:K28">_xlfn.ANCHORARRAY(C18)=K2:N12</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I18" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J18" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K18" t="e" vm="2">
+        <v>#VALUE!</v>
       </c>
       <c r="M18" s="11" t="s">
         <v>15</v>
@@ -20471,21 +20559,17 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="5"/>
-      <c r="H19" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I19" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J19" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K19" t="b">
-        <f ca="1"/>
-        <v>1</v>
+      <c r="H19" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I19" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J19" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K19" t="e" vm="2">
+        <v>#VALUE!</v>
       </c>
       <c r="M19" s="11"/>
       <c r="P19" s="8"/>
@@ -20496,21 +20580,17 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="H20" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I20" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J20" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K20" t="b">
-        <f ca="1"/>
-        <v>1</v>
+      <c r="H20" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I20" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J20" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K20" t="e" vm="2">
+        <v>#VALUE!</v>
       </c>
       <c r="M20" s="11" t="s">
         <v>14</v>
@@ -20523,21 +20603,17 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="H21" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I21" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J21" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K21" t="b">
-        <f ca="1"/>
-        <v>1</v>
+      <c r="H21" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I21" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J21" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K21" t="e" vm="2">
+        <v>#VALUE!</v>
       </c>
       <c r="M21" s="11"/>
       <c r="P21" s="8"/>
@@ -20548,21 +20624,17 @@
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
       <c r="F22" s="4"/>
-      <c r="H22" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I22" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J22" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K22" t="b">
-        <f ca="1"/>
-        <v>1</v>
+      <c r="H22" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I22" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J22" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K22" t="e" vm="2">
+        <v>#VALUE!</v>
       </c>
       <c r="P22" s="8"/>
       <c r="S22" s="9"/>
@@ -20572,21 +20644,17 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="5"/>
-      <c r="H23" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I23" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J23" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K23" t="b">
-        <f ca="1"/>
-        <v>1</v>
+      <c r="H23" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I23" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J23" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K23" t="e" vm="2">
+        <v>#VALUE!</v>
       </c>
       <c r="N23" s="11" t="s">
         <v>16</v>
@@ -20599,21 +20667,17 @@
       <c r="D24" s="5"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="H24" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I24" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J24" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K24" t="b">
-        <f ca="1"/>
-        <v>1</v>
+      <c r="H24" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I24" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J24" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K24" t="e" vm="2">
+        <v>#VALUE!</v>
       </c>
       <c r="N24" s="11" t="str" cm="1">
         <f t="array" ref="N24">INDEX(C2:F12,ROW(C24)+2-ROW(C18)+1,COLUMN(C24)+2-COLUMN(C18)+1)</f>
@@ -20627,21 +20691,17 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="H25" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I25" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J25" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K25" t="b">
-        <f ca="1"/>
-        <v>1</v>
+      <c r="H25" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I25" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J25" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K25" t="e" vm="2">
+        <v>#VALUE!</v>
       </c>
       <c r="O25">
         <f>COLUMN(N23)</f>
@@ -20655,21 +20715,17 @@
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
       <c r="F26" s="4"/>
-      <c r="H26" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I26" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J26" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K26" t="b">
-        <f ca="1"/>
-        <v>1</v>
+      <c r="H26" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I26" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J26" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K26" t="e" vm="2">
+        <v>#VALUE!</v>
       </c>
       <c r="P26" s="8"/>
       <c r="S26" s="9"/>
@@ -20679,21 +20735,17 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="H27" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I27" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J27" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K27" t="b">
-        <f ca="1"/>
-        <v>1</v>
+      <c r="H27" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I27" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J27" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K27" t="e" vm="2">
+        <v>#VALUE!</v>
       </c>
       <c r="P27" s="8"/>
       <c r="S27" s="9"/>
@@ -20703,21 +20755,17 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="H28" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="I28" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="J28" t="b">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="K28" t="b">
-        <f ca="1"/>
-        <v>1</v>
+      <c r="H28" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I28" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J28" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K28" t="e" vm="2">
+        <v>#VALUE!</v>
       </c>
       <c r="P28" s="8"/>
       <c r="S28" s="9"/>

</xml_diff>

<commit_message>
My interim is getting close
</commit_message>
<xml_diff>
--- a/CH-92 Missing value.xlsx
+++ b/CH-92 Missing value.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D284A7E-211F-414D-979A-055A89E029FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5F5A09-AED1-4F51-B190-3832A6B51F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,9 +44,8 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="2">
+  <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -57,35 +56,11 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="2">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="1"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="2">
-    <bk>
-      <rc t="2" v="0"/>
-    </bk>
-    <bk>
-      <rc t="2" v="1"/>
-    </bk>
-  </valueMetadata>
 </metadata>
 </file>
 
@@ -731,72 +706,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
-  <rv s="0">
-    <v>13</v>
-    <v>2</v>
-  </rv>
-  <rv s="1">
-    <v>13</v>
-    <v>1</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
-  <s t="_error">
-    <k n="errorType" t="i"/>
-    <k n="subType" t="i"/>
-  </s>
-  <s t="_error">
-    <k n="errorType" t="i"/>
-    <k n="propagated" t="b"/>
-  </s>
-</rvStructures>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -19959,8 +19868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A932BE-8E3C-470C-A0EC-77638493AE59}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -20522,32 +20431,38 @@
       <c r="S17" s="9"/>
     </row>
     <row r="18" spans="3:19" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C18" s="3" t="e" cm="1" vm="1">
-        <f t="array" ref="C18">_xlfn.VSTACK(K2:N2,_xlfn.MAP(
+      <c r="C18" s="3" t="str" cm="1">
+        <f t="array" ref="C18:F28">_xlfn.VSTACK(K2:N2,_xlfn.MAP(
 C3:F12,
 _xlfn.LAMBDA(_xlpm.v,_xlfn.LET(_xlpm.r,_xlfn.IFS(_xlpm.v="U",-1,_xlpm.v="D",1,1,0),
 _xlpm.c,_xlfn.IFS(_xlpm.v="L",-1,_xlpm.v="R",1,1,0),
 _xlpm.z,INDEX(_xlpm.v,1,1):INDEX(_xlpm.v,1,1),
-INDEX($C$3:$F$12,ROW(_xlpm.z)+_xlpm.r-3,COLUMN(_xlpm.z)+_xlpm.c-3)
+_xlfn.TEXTJOIN("|",,ROW(_xlpm.z)+_xlpm.r-3+1,COLUMN(_xlpm.z)+_xlpm.c-3+1)
 )
 )))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="H18" t="e" cm="1" vm="2">
+        <v>Row ID</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <v>X</v>
+      </c>
+      <c r="E18" s="3" t="str">
+        <v>Y</v>
+      </c>
+      <c r="F18" s="3" t="str">
+        <v>Z</v>
+      </c>
+      <c r="H18" t="b" cm="1">
         <f t="array" ref="H18:K28">_xlfn.ANCHORARRAY(C18)=K2:N12</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I18" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J18" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K18" t="e" vm="2">
-        <v>#VALUE!</v>
+        <v>1</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" t="b">
+        <v>1</v>
       </c>
       <c r="M18" s="11" t="s">
         <v>15</v>
@@ -20555,42 +20470,58 @@
       <c r="S18" s="9"/>
     </row>
     <row r="19" spans="3:19" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
-      <c r="H19" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I19" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J19" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K19" t="e" vm="2">
-        <v>#VALUE!</v>
+      <c r="C19" s="4" t="str">
+        <v>1|1</v>
+      </c>
+      <c r="D19" s="4" t="str">
+        <v>1|2</v>
+      </c>
+      <c r="E19" s="4" t="str">
+        <v>1|3</v>
+      </c>
+      <c r="F19" s="5" t="str">
+        <v>0|4</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="b">
+        <v>0</v>
       </c>
       <c r="M19" s="11"/>
       <c r="P19" s="8"/>
       <c r="S19" s="9"/>
     </row>
     <row r="20" spans="3:19" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="H20" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I20" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J20" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K20" t="e" vm="2">
-        <v>#VALUE!</v>
+      <c r="C20" s="4" t="str">
+        <v>2|1</v>
+      </c>
+      <c r="D20" s="4" t="str">
+        <v>2|2</v>
+      </c>
+      <c r="E20" s="4" t="str">
+        <v>2|3</v>
+      </c>
+      <c r="F20" s="4" t="str">
+        <v>2|4</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <v>0</v>
       </c>
       <c r="M20" s="11" t="s">
         <v>14</v>
@@ -20599,62 +20530,86 @@
       <c r="S20" s="9"/>
     </row>
     <row r="21" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="H21" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I21" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J21" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K21" t="e" vm="2">
-        <v>#VALUE!</v>
+      <c r="C21" s="4" t="str">
+        <v>3|1</v>
+      </c>
+      <c r="D21" s="4" t="str">
+        <v>3|2</v>
+      </c>
+      <c r="E21" s="4" t="str">
+        <v>3|3</v>
+      </c>
+      <c r="F21" s="4" t="str">
+        <v>3|4</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
+        <v>0</v>
       </c>
       <c r="M21" s="11"/>
       <c r="P21" s="8"/>
       <c r="S21" s="9"/>
     </row>
     <row r="22" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="4"/>
-      <c r="H22" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I22" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J22" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K22" t="e" vm="2">
-        <v>#VALUE!</v>
+      <c r="C22" s="4" t="str">
+        <v>4|1</v>
+      </c>
+      <c r="D22" s="4" t="str">
+        <v>4|2</v>
+      </c>
+      <c r="E22" s="5" t="str">
+        <v>5|3</v>
+      </c>
+      <c r="F22" s="4" t="str">
+        <v>4|4</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="b">
+        <v>0</v>
       </c>
       <c r="P22" s="8"/>
       <c r="S22" s="9"/>
     </row>
     <row r="23" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
-      <c r="H23" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I23" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J23" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K23" t="e" vm="2">
-        <v>#VALUE!</v>
+      <c r="C23" s="4" t="str">
+        <v>5|1</v>
+      </c>
+      <c r="D23" s="4" t="str">
+        <v>5|2</v>
+      </c>
+      <c r="E23" s="4" t="str">
+        <v>5|3</v>
+      </c>
+      <c r="F23" s="5" t="str">
+        <v>5|3</v>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="b">
+        <v>0</v>
       </c>
       <c r="N23" s="11" t="s">
         <v>16</v>
@@ -20663,21 +20618,29 @@
       <c r="S23" s="9"/>
     </row>
     <row r="24" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="H24" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I24" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J24" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K24" t="e" vm="2">
-        <v>#VALUE!</v>
+      <c r="C24" s="4" t="str">
+        <v>6|1</v>
+      </c>
+      <c r="D24" s="5" t="str">
+        <v>6|3</v>
+      </c>
+      <c r="E24" s="4" t="str">
+        <v>6|3</v>
+      </c>
+      <c r="F24" s="4" t="str">
+        <v>6|4</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
+        <v>0</v>
       </c>
       <c r="N24" s="11" t="str" cm="1">
         <f t="array" ref="N24">INDEX(C2:F12,ROW(C24)+2-ROW(C18)+1,COLUMN(C24)+2-COLUMN(C18)+1)</f>
@@ -20687,21 +20650,29 @@
       <c r="S24" s="9"/>
     </row>
     <row r="25" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="H25" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I25" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J25" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K25" t="e" vm="2">
-        <v>#VALUE!</v>
+      <c r="C25" s="4" t="str">
+        <v>7|1</v>
+      </c>
+      <c r="D25" s="4" t="str">
+        <v>7|2</v>
+      </c>
+      <c r="E25" s="4" t="str">
+        <v>7|3</v>
+      </c>
+      <c r="F25" s="4" t="str">
+        <v>7|4</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="b">
+        <v>0</v>
       </c>
       <c r="O25">
         <f>COLUMN(N23)</f>
@@ -20711,61 +20682,85 @@
       <c r="S25" s="9"/>
     </row>
     <row r="26" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="4"/>
-      <c r="H26" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I26" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J26" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K26" t="e" vm="2">
-        <v>#VALUE!</v>
+      <c r="C26" s="4" t="str">
+        <v>8|1</v>
+      </c>
+      <c r="D26" s="4" t="str">
+        <v>8|2</v>
+      </c>
+      <c r="E26" s="5" t="str">
+        <v>8|2</v>
+      </c>
+      <c r="F26" s="4" t="str">
+        <v>8|4</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="b">
+        <v>0</v>
       </c>
       <c r="P26" s="8"/>
       <c r="S26" s="9"/>
     </row>
     <row r="27" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="H27" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I27" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J27" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K27" t="e" vm="2">
-        <v>#VALUE!</v>
+      <c r="C27" s="4" t="str">
+        <v>9|1</v>
+      </c>
+      <c r="D27" s="4" t="str">
+        <v>9|2</v>
+      </c>
+      <c r="E27" s="4" t="str">
+        <v>9|3</v>
+      </c>
+      <c r="F27" s="4" t="str">
+        <v>9|4</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" t="b">
+        <v>0</v>
       </c>
       <c r="P27" s="8"/>
       <c r="S27" s="9"/>
     </row>
     <row r="28" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="H28" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I28" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J28" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K28" t="e" vm="2">
-        <v>#VALUE!</v>
+      <c r="C28" s="4" t="str">
+        <v>10|1</v>
+      </c>
+      <c r="D28" s="4" t="str">
+        <v>10|2</v>
+      </c>
+      <c r="E28" s="4" t="str">
+        <v>10|3</v>
+      </c>
+      <c r="F28" s="4" t="str">
+        <v>10|4</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" t="b">
+        <v>0</v>
       </c>
       <c r="P28" s="8"/>
       <c r="S28" s="9"/>

</xml_diff>